<commit_message>
AddCustomerTest and Excel file reader executed
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -7,10 +7,33 @@
     <workbookView windowWidth="22188" windowHeight="9024"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Sagrika</t>
+  </si>
+  <si>
+    <t>Srivastava</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,6 +649,9 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1161,14 +1187,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Open Account Test Executed successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>firstname</t>
   </si>
@@ -37,7 +38,28 @@
     <t>001100</t>
   </si>
   <si>
-    <t>ustomer added successfully</t>
+    <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>Shubhi</t>
+  </si>
+  <si>
+    <t>Utkarsh</t>
+  </si>
+  <si>
+    <t>Geetika</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Sagrika Srivastava</t>
+  </si>
+  <si>
+    <t>Rupee</t>
   </si>
 </sst>
 </file>
@@ -1193,13 +1215,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
     <col min="4" max="4" width="25.6666666666667" customWidth="1"/>
   </cols>
@@ -1232,6 +1254,81 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>